<commit_message>
adding pseudo instruction tab
</commit_message>
<xml_diff>
--- a/LEVEL1/BasicRISCInstTable.xlsx
+++ b/LEVEL1/BasicRISCInstTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleidel/dev/working/GHCoregenTutorials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleidel/dev/working/GHCoregenTutorials/LEVEL1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0685E36D-2564-5442-8CD0-4D3CFE559722}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9765FE17-2110-0546-885D-E808B242649C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="2660" windowWidth="25940" windowHeight="17480" xr2:uid="{923FD8C1-503B-724C-81C7-28A7050BB589}"/>
+    <workbookView xWindow="18080" yWindow="3140" windowWidth="19480" windowHeight="17480" firstSheet="4" activeTab="11" xr2:uid="{923FD8C1-503B-724C-81C7-28A7050BB589}"/>
   </bookViews>
   <sheets>
     <sheet name="Coversheet" sheetId="3" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="OPC=0x0A" sheetId="10" r:id="rId9"/>
     <sheet name="OPC=0x11" sheetId="8" r:id="rId10"/>
     <sheet name="OPC=0x12" sheetId="11" r:id="rId11"/>
+    <sheet name="PseudoInsts" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="167">
   <si>
     <t>Opcode</t>
   </si>
@@ -484,10 +485,58 @@
     <t>Copyright 2018, 2019 Tactical Computing Laboratories, LLC; See LICENSE for licensing details</t>
   </si>
   <si>
-    <t xml:space="preserve">This document contains the encoding infrastructure for the BasicRISC instruction set architecture detailed in the System Architect Level1 Tutorial.  The opcode classes are listed in the "Opcode" sheet.  For each opcode class that is defined, a separate sheet is present that defines the associated function (func) codes and the associated instructions with their respective mnemonics.  </t>
-  </si>
-  <si>
     <t>BasicRISCInstTable: System Architect BasicRISC instruction set encoding tables: Level 1 v.1.0</t>
+  </si>
+  <si>
+    <t>Base Instruction Mnemonic</t>
+  </si>
+  <si>
+    <t>Pseudo Instruction Mnemonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This document contains the encoding infrastructure for the BasicRISC instruction set architecture detailed in the System Architect Level1 Tutorial.  The opcode classes are listed in the "Opcode" sheet.  For each opcode class that is defined, a separate sheet is present that defines the associated function (func) codes and the associated instructions with their respective mnemonics.  Finally, the PseudoInsts tab provides pseudo instruction mnemonics with their equivalent base encodings  </t>
+  </si>
+  <si>
+    <t>Size (bytes)</t>
+  </si>
+  <si>
+    <t>unsigned byte</t>
+  </si>
+  <si>
+    <t>unsigned halfword</t>
+  </si>
+  <si>
+    <t>unsigned word</t>
+  </si>
+  <si>
+    <t>unsigned doubleword</t>
+  </si>
+  <si>
+    <t>signed byte</t>
+  </si>
+  <si>
+    <t>signed halfword</t>
+  </si>
+  <si>
+    <t>signed word</t>
+  </si>
+  <si>
+    <t>signed doubleword</t>
+  </si>
+  <si>
+    <t>Mnemonic</t>
+  </si>
+  <si>
+    <t>MOV RT, RA</t>
+  </si>
+  <si>
+    <t>ADD RT, RA, R0</t>
+  </si>
+  <si>
+    <t>MOVCG RT,RA</t>
+  </si>
+  <si>
+    <t>MOVGC RT,RA</t>
   </si>
 </sst>
 </file>
@@ -942,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,19 +1047,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1022,6 +1059,87 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1040,86 +1158,34 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1490,130 +1556,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2411AE6A-16D0-CE4A-B5B3-581F688B992D}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="57"/>
+      <c r="A1" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="29"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="60"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="58"/>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="60"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="60"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="58"/>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="60"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="60"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="32"/>
     </row>
     <row r="7" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="63"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="35"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="36" t="s">
         <v>148</v>
       </c>
       <c r="B8" s="37"/>
@@ -1628,401 +1697,460 @@
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
       <c r="M8" s="37"/>
-      <c r="N8" s="39"/>
+      <c r="N8" s="38"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="42"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="42"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="41"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="42"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="41"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="42"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="41"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="41"/>
     </row>
     <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-      <c r="N15" s="45"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="44"/>
     </row>
     <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="48"/>
+      <c r="A18" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="47"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="49"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="51"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="50"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="49"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="51"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="50"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="49"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="51"/>
+      <c r="A21" s="48"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="51"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="50"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="49"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="51"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="49"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="51"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="50"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="51"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="51"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="49"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="51"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="49"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
-      <c r="L29" s="50"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="51"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="50"/>
-      <c r="N30" s="51"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="50"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="51"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="50"/>
     </row>
     <row r="32" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="53"/>
-      <c r="M32" s="53"/>
-      <c r="N32" s="54"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A32" s="51"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="53"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D37" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D38" s="69" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="E38" s="69">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D39" s="69" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="E39" s="69">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D40" s="69" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="E40" s="69">
+        <v>4</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D41" s="69" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="E41" s="69">
+        <v>8</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D42" s="69" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="E42" s="69">
+        <v>1</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D43" s="69" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="E43" s="69">
+        <v>2</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D44" s="69" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="E44" s="69">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D45" s="69" t="s">
         <v>36</v>
+      </c>
+      <c r="E45" s="69">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2041,7 +2169,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2052,14 +2180,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -2117,13 +2245,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2149,7 +2277,7 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2344,14 +2472,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -2409,13 +2537,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2441,7 +2569,7 @@
       <c r="G5" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="22" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2616,6 +2744,161 @@
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B4:G4"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D682C20-5D66-8440-823B-FBE572026D57}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="64"/>
+      <c r="B1" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="66" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="70"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2646,152 +2929,152 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="27">
+      <c r="A2" s="23">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="54" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="29">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="55"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="29">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="55"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="29">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C5" s="32"/>
+      <c r="C5" s="55"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="29">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="55"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="29">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="55"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="29">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="29">
+      <c r="A9" s="25">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="55"/>
     </row>
     <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C10" s="33"/>
+      <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="27">
+      <c r="A11" s="23">
         <v>9</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="57" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="29">
+      <c r="A12" s="25">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C12" s="35"/>
+      <c r="C12" s="58"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="29">
+      <c r="A13" s="25">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="58"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="29">
+      <c r="A14" s="25">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="58"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="29">
+      <c r="A15" s="25">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="58"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="29">
+      <c r="A16" s="25">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="58"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="29">
+      <c r="A17" s="25">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="58"/>
     </row>
     <row r="18" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2800,72 +3083,72 @@
       <c r="B18" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="59"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="27">
+      <c r="A19" s="23">
         <v>17</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="54" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="29">
+      <c r="A20" s="25">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="32"/>
+      <c r="C20" s="55"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="29">
+      <c r="A21" s="25">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="32"/>
+      <c r="C21" s="55"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="29">
+      <c r="A22" s="25">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="32"/>
+      <c r="C22" s="55"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="29">
+      <c r="A23" s="25">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="32"/>
+      <c r="C23" s="55"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="29">
+      <c r="A24" s="25">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C24" s="32"/>
+      <c r="C24" s="55"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="29">
+      <c r="A25" s="25">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C25" s="32"/>
+      <c r="C25" s="55"/>
     </row>
     <row r="26" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -2874,72 +3157,72 @@
       <c r="B26" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="33"/>
+      <c r="C26" s="56"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="27">
+      <c r="A27" s="23">
         <v>25</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="57" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="29">
+      <c r="A28" s="25">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="35"/>
+      <c r="C28" s="58"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="29">
+      <c r="A29" s="25">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="35"/>
+      <c r="C29" s="58"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="29">
+      <c r="A30" s="25">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C30" s="35"/>
+      <c r="C30" s="58"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="29">
+      <c r="A31" s="25">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C31" s="35"/>
+      <c r="C31" s="58"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="29">
+      <c r="A32" s="25">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="35"/>
+      <c r="C32" s="58"/>
     </row>
     <row r="33" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="36"/>
+      <c r="C33" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2957,7 +3240,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2968,14 +3251,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -3033,13 +3316,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3452,14 +3735,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -3517,13 +3800,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3824,14 +4107,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -3889,13 +4172,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4324,14 +4607,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -4389,13 +4672,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4605,7 +4888,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4616,14 +4899,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -4681,13 +4964,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4913,7 +5196,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4924,14 +5207,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -4989,13 +5272,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5021,7 +5304,7 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="22" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5205,7 +5488,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B2" sqref="B2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5216,14 +5499,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -5281,13 +5564,13 @@
       <c r="A4" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="21" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5313,7 +5596,7 @@
       <c r="G5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="22" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5339,7 +5622,7 @@
       <c r="G6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="22" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed RA to [4-0] in xlsx; made PC RW in BasicRISC.yaml; Corrected PPTX slide 35
</commit_message>
<xml_diff>
--- a/LEVEL1/BasicRISCInstTable.xlsx
+++ b/LEVEL1/BasicRISCInstTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleidel/dev/working/GHCoregenTutorials/LEVEL1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brick/brick-dev/CoreGenTutorials/LEVEL1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179CFC59-431C-914C-B396-9BCAB80EE3AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847645BB-16B4-2443-897E-6CC86C8714DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="2540" windowWidth="25040" windowHeight="17500" firstSheet="4" activeTab="11" xr2:uid="{923FD8C1-503B-724C-81C7-28A7050BB589}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" firstSheet="4" activeTab="11" xr2:uid="{923FD8C1-503B-724C-81C7-28A7050BB589}"/>
   </bookViews>
   <sheets>
     <sheet name="Coversheet" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="170">
   <si>
     <t>Opcode</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>LADD CTRL, R0, RB</t>
+  </si>
+  <si>
+    <t>[4-0]</t>
   </si>
 </sst>
 </file>
@@ -2761,8 +2764,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2791,7 +2794,7 @@
         <v>24</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>